<commit_message>
check data if want import data change exist CNN
</commit_message>
<xml_diff>
--- a/XettuyenDGNLTHPT/UploadCNN.xlsx
+++ b/XettuyenDGNLTHPT/UploadCNN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BDAEA97D-E376-4E28-AE45-9ED04EADCE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33392C75-3E10-4AA8-B995-2C37B230451D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11835" yWindow="3420" windowWidth="15660" windowHeight="12270" xr2:uid="{032AA657-87AE-4119-87B9-42B293C12097}"/>
+    <workbookView xWindow="9120" yWindow="3000" windowWidth="15660" windowHeight="12270" xr2:uid="{032AA657-87AE-4119-87B9-42B293C12097}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,6 +444,9 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>